<commit_message>
Items.xlsx add category tag
</commit_message>
<xml_diff>
--- a/Items.xlsx
+++ b/Items.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
-  <workbookPr defaultThemeVersion="202300"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20415"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\곰치\Desktop\TFI\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bagja\Desktop\TFIGIT\DisasterioTest\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23D2ED62-499F-4B70-8254-8EE4D2E7D8A6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA5A0A23-8D32-4C7C-8D9D-CB1E8D02A07F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="12315" yWindow="3075" windowWidth="21600" windowHeight="11385" xr2:uid="{5E2D2B26-9E3D-45A7-9237-86961CAF8455}"/>
+    <workbookView xWindow="12320" yWindow="3080" windowWidth="21600" windowHeight="11390" xr2:uid="{5E2D2B26-9E3D-45A7-9237-86961CAF8455}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,10 +25,10 @@
         <xcalcf:feature name="microsoft.com:RD"/>
         <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="151">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="305" uniqueCount="171">
   <si>
     <t>laptop</t>
   </si>
@@ -1257,6 +1257,66 @@
   <si>
     <t>description</t>
     <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>tag</t>
+  </si>
+  <si>
+    <t>korTag</t>
+  </si>
+  <si>
+    <t>personal_care</t>
+  </si>
+  <si>
+    <t>개인위생/관리용품</t>
+  </si>
+  <si>
+    <t>clothing</t>
+  </si>
+  <si>
+    <t>의류</t>
+  </si>
+  <si>
+    <t>baby</t>
+  </si>
+  <si>
+    <t>유아용품</t>
+  </si>
+  <si>
+    <t>stationery</t>
+  </si>
+  <si>
+    <t>문구류</t>
+  </si>
+  <si>
+    <t>food</t>
+  </si>
+  <si>
+    <t>식품</t>
+  </si>
+  <si>
+    <t>medical</t>
+  </si>
+  <si>
+    <t>의약/의료</t>
+  </si>
+  <si>
+    <t>baby,food</t>
+  </si>
+  <si>
+    <t>유아용품,식품</t>
+  </si>
+  <si>
+    <t>electronics</t>
+  </si>
+  <si>
+    <t>전자기기</t>
+  </si>
+  <si>
+    <t>baby,clothing</t>
+  </si>
+  <si>
+    <t>유아용품,의류</t>
   </si>
 </sst>
 </file>
@@ -1665,15 +1725,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DAD4C3C8-9C96-49F8-8571-F20EA12BCCB9}">
-  <dimension ref="A1:E75"/>
+  <dimension ref="A1:G75"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="17" x14ac:dyDescent="0.45"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A1" s="3" t="s">
         <v>146</v>
       </c>
@@ -1689,8 +1749,14 @@
       <c r="E1" s="2" t="s">
         <v>150</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F1" t="s">
+        <v>151</v>
+      </c>
+      <c r="G1" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A2" s="1" t="s">
         <v>143</v>
       </c>
@@ -1706,8 +1772,14 @@
       <c r="E2" t="s">
         <v>144</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F2" t="s">
+        <v>153</v>
+      </c>
+      <c r="G2" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A3" s="1" t="s">
         <v>141</v>
       </c>
@@ -1723,8 +1795,14 @@
       <c r="E3" t="s">
         <v>145</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F3" t="s">
+        <v>155</v>
+      </c>
+      <c r="G3" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A4" s="1" t="s">
         <v>139</v>
       </c>
@@ -1737,8 +1815,14 @@
       <c r="D4" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F4" t="s">
+        <v>153</v>
+      </c>
+      <c r="G4" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A5" s="1" t="s">
         <v>137</v>
       </c>
@@ -1751,8 +1835,14 @@
       <c r="D5" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F5" t="s">
+        <v>153</v>
+      </c>
+      <c r="G5" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A6" s="1" t="s">
         <v>135</v>
       </c>
@@ -1765,8 +1855,14 @@
       <c r="D6" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F6" t="s">
+        <v>157</v>
+      </c>
+      <c r="G6" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A7" s="1" t="s">
         <v>133</v>
       </c>
@@ -1779,8 +1875,14 @@
       <c r="D7" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F7" t="s">
+        <v>155</v>
+      </c>
+      <c r="G7" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A8" s="1" t="s">
         <v>131</v>
       </c>
@@ -1793,8 +1895,14 @@
       <c r="D8" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F8" t="s">
+        <v>153</v>
+      </c>
+      <c r="G8" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A9" s="1" t="s">
         <v>129</v>
       </c>
@@ -1807,8 +1915,14 @@
       <c r="D9" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F9" t="s">
+        <v>159</v>
+      </c>
+      <c r="G9" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A10" s="1" t="s">
         <v>127</v>
       </c>
@@ -1821,8 +1935,14 @@
       <c r="D10" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F10" t="s">
+        <v>159</v>
+      </c>
+      <c r="G10" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A11" s="1" t="s">
         <v>125</v>
       </c>
@@ -1835,8 +1955,14 @@
       <c r="D11" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F11" t="s">
+        <v>153</v>
+      </c>
+      <c r="G11" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A12" s="1" t="s">
         <v>123</v>
       </c>
@@ -1849,8 +1975,14 @@
       <c r="D12" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F12" t="s">
+        <v>153</v>
+      </c>
+      <c r="G12" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A13" s="1" t="s">
         <v>121</v>
       </c>
@@ -1863,8 +1995,14 @@
       <c r="D13" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F13" t="s">
+        <v>161</v>
+      </c>
+      <c r="G13" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A14" s="1" t="s">
         <v>119</v>
       </c>
@@ -1877,8 +2015,14 @@
       <c r="D14" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F14" t="s">
+        <v>161</v>
+      </c>
+      <c r="G14" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A15" s="1" t="s">
         <v>117</v>
       </c>
@@ -1891,8 +2035,14 @@
       <c r="D15" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F15" t="s">
+        <v>155</v>
+      </c>
+      <c r="G15" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A16" s="1" t="s">
         <v>116</v>
       </c>
@@ -1905,8 +2055,14 @@
       <c r="D16" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="F16" t="s">
+        <v>163</v>
+      </c>
+      <c r="G16" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A17" s="1" t="s">
         <v>114</v>
       </c>
@@ -1919,8 +2075,14 @@
       <c r="D17" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="F17" t="s">
+        <v>165</v>
+      </c>
+      <c r="G17" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A18" s="1" t="s">
         <v>112</v>
       </c>
@@ -1933,8 +2095,14 @@
       <c r="D18" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="F18" t="s">
+        <v>161</v>
+      </c>
+      <c r="G18" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A19" s="1" t="s">
         <v>110</v>
       </c>
@@ -1947,8 +2115,14 @@
       <c r="D19" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="F19" t="s">
+        <v>155</v>
+      </c>
+      <c r="G19" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A20" s="1" t="s">
         <v>108</v>
       </c>
@@ -1961,8 +2135,14 @@
       <c r="D20" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="F20" t="s">
+        <v>161</v>
+      </c>
+      <c r="G20" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A21" s="1" t="s">
         <v>92</v>
       </c>
@@ -1975,8 +2155,14 @@
       <c r="D21" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="F21" t="s">
+        <v>163</v>
+      </c>
+      <c r="G21" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A22" s="1" t="s">
         <v>106</v>
       </c>
@@ -1989,8 +2175,14 @@
       <c r="D22" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="F22" t="s">
+        <v>153</v>
+      </c>
+      <c r="G22" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A23" s="1" t="s">
         <v>104</v>
       </c>
@@ -2003,8 +2195,14 @@
       <c r="D23" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="F23" t="s">
+        <v>161</v>
+      </c>
+      <c r="G23" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A24" s="1" t="s">
         <v>102</v>
       </c>
@@ -2017,8 +2215,14 @@
       <c r="D24" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="F24" t="s">
+        <v>167</v>
+      </c>
+      <c r="G24" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A25" s="1" t="s">
         <v>100</v>
       </c>
@@ -2031,8 +2235,14 @@
       <c r="D25" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="F25" t="s">
+        <v>155</v>
+      </c>
+      <c r="G25" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A26" s="1" t="s">
         <v>98</v>
       </c>
@@ -2045,8 +2255,14 @@
       <c r="D26" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="F26" t="s">
+        <v>155</v>
+      </c>
+      <c r="G26" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A27" s="1" t="s">
         <v>96</v>
       </c>
@@ -2059,8 +2275,14 @@
       <c r="D27" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="F27" t="s">
+        <v>153</v>
+      </c>
+      <c r="G27" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A28" s="1" t="s">
         <v>94</v>
       </c>
@@ -2073,8 +2295,14 @@
       <c r="D28" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="F28" t="s">
+        <v>169</v>
+      </c>
+      <c r="G28" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A29" s="1" t="s">
         <v>92</v>
       </c>
@@ -2087,8 +2315,14 @@
       <c r="D29" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="F29" t="s">
+        <v>163</v>
+      </c>
+      <c r="G29" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A30" s="1" t="s">
         <v>90</v>
       </c>
@@ -2101,8 +2335,14 @@
       <c r="D30" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="F30" t="s">
+        <v>161</v>
+      </c>
+      <c r="G30" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A31" s="1" t="s">
         <v>88</v>
       </c>
@@ -2115,8 +2355,14 @@
       <c r="D31" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="F31" t="s">
+        <v>155</v>
+      </c>
+      <c r="G31" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A32" s="1" t="s">
         <v>86</v>
       </c>
@@ -2129,8 +2375,14 @@
       <c r="D32" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="F32" t="s">
+        <v>159</v>
+      </c>
+      <c r="G32" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A33" s="1" t="s">
         <v>84</v>
       </c>
@@ -2143,8 +2395,14 @@
       <c r="D33" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="F33" t="s">
+        <v>159</v>
+      </c>
+      <c r="G33" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A34" s="1" t="s">
         <v>82</v>
       </c>
@@ -2157,8 +2415,14 @@
       <c r="D34" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="F34" t="s">
+        <v>155</v>
+      </c>
+      <c r="G34" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A35" s="1" t="s">
         <v>80</v>
       </c>
@@ -2171,8 +2435,14 @@
       <c r="D35" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="F35" t="s">
+        <v>153</v>
+      </c>
+      <c r="G35" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A36" s="1" t="s">
         <v>78</v>
       </c>
@@ -2185,8 +2455,14 @@
       <c r="D36" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="F36" t="s">
+        <v>167</v>
+      </c>
+      <c r="G36" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A37" s="1" t="s">
         <v>76</v>
       </c>
@@ -2199,8 +2475,14 @@
       <c r="D37" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="F37" t="s">
+        <v>155</v>
+      </c>
+      <c r="G37" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A38" s="1" t="s">
         <v>74</v>
       </c>
@@ -2213,8 +2495,14 @@
       <c r="D38" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="F38" t="s">
+        <v>155</v>
+      </c>
+      <c r="G38" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A39" s="1" t="s">
         <v>72</v>
       </c>
@@ -2227,8 +2515,14 @@
       <c r="D39" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="F39" t="s">
+        <v>155</v>
+      </c>
+      <c r="G39" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A40" s="1" t="s">
         <v>70</v>
       </c>
@@ -2241,8 +2535,14 @@
       <c r="D40" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="F40" t="s">
+        <v>161</v>
+      </c>
+      <c r="G40" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A41" s="1" t="s">
         <v>68</v>
       </c>
@@ -2255,8 +2555,14 @@
       <c r="D41" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="F41" t="s">
+        <v>161</v>
+      </c>
+      <c r="G41" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A42" s="1" t="s">
         <v>67</v>
       </c>
@@ -2269,8 +2575,14 @@
       <c r="D42" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="F42" t="s">
+        <v>155</v>
+      </c>
+      <c r="G42" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A43" s="1" t="s">
         <v>65</v>
       </c>
@@ -2283,8 +2595,14 @@
       <c r="D43" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="F43" t="s">
+        <v>167</v>
+      </c>
+      <c r="G43" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A44" s="1" t="s">
         <v>63</v>
       </c>
@@ -2297,8 +2615,14 @@
       <c r="D44" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="F44" t="s">
+        <v>153</v>
+      </c>
+      <c r="G44" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A45" s="1" t="s">
         <v>61</v>
       </c>
@@ -2311,8 +2635,14 @@
       <c r="D45" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="F45" t="s">
+        <v>161</v>
+      </c>
+      <c r="G45" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A46" s="1" t="s">
         <v>59</v>
       </c>
@@ -2325,8 +2655,14 @@
       <c r="D46" s="1">
         <v>2</v>
       </c>
-    </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="F46" t="s">
+        <v>153</v>
+      </c>
+      <c r="G46" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A47" s="1" t="s">
         <v>57</v>
       </c>
@@ -2339,8 +2675,14 @@
       <c r="D47" s="1">
         <v>2</v>
       </c>
-    </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="F47" t="s">
+        <v>159</v>
+      </c>
+      <c r="G47" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A48" s="1" t="s">
         <v>55</v>
       </c>
@@ -2353,8 +2695,14 @@
       <c r="D48" s="1">
         <v>2</v>
       </c>
-    </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="F48" t="s">
+        <v>155</v>
+      </c>
+      <c r="G48" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="49" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A49" s="1" t="s">
         <v>53</v>
       </c>
@@ -2367,8 +2715,14 @@
       <c r="D49" s="1">
         <v>2</v>
       </c>
-    </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="F49" t="s">
+        <v>157</v>
+      </c>
+      <c r="G49" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="50" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A50" s="1" t="s">
         <v>51</v>
       </c>
@@ -2381,8 +2735,14 @@
       <c r="D50" s="1">
         <v>2</v>
       </c>
-    </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="F50" t="s">
+        <v>161</v>
+      </c>
+      <c r="G50" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="51" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A51" s="1" t="s">
         <v>49</v>
       </c>
@@ -2395,8 +2755,14 @@
       <c r="D51" s="1">
         <v>2</v>
       </c>
-    </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="F51" t="s">
+        <v>157</v>
+      </c>
+      <c r="G51" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="52" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A52" s="1" t="s">
         <v>47</v>
       </c>
@@ -2409,8 +2775,14 @@
       <c r="D52" s="1">
         <v>2</v>
       </c>
-    </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="F52" t="s">
+        <v>153</v>
+      </c>
+      <c r="G52" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="53" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A53" s="1" t="s">
         <v>45</v>
       </c>
@@ -2423,8 +2795,14 @@
       <c r="D53" s="1">
         <v>2</v>
       </c>
-    </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="F53" t="s">
+        <v>161</v>
+      </c>
+      <c r="G53" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="54" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A54" s="1" t="s">
         <v>43</v>
       </c>
@@ -2437,8 +2815,14 @@
       <c r="D54" s="1">
         <v>2</v>
       </c>
-    </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="F54" t="s">
+        <v>163</v>
+      </c>
+      <c r="G54" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="55" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A55" s="1" t="s">
         <v>41</v>
       </c>
@@ -2451,8 +2835,14 @@
       <c r="D55" s="1">
         <v>2</v>
       </c>
-    </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="F55" t="s">
+        <v>155</v>
+      </c>
+      <c r="G55" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="56" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A56" s="1" t="s">
         <v>39</v>
       </c>
@@ -2465,8 +2855,14 @@
       <c r="D56" s="1">
         <v>2</v>
       </c>
-    </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="F56" t="s">
+        <v>167</v>
+      </c>
+      <c r="G56" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="57" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A57" s="1" t="s">
         <v>37</v>
       </c>
@@ -2479,8 +2875,14 @@
       <c r="D57" s="1">
         <v>2</v>
       </c>
-    </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="F57" t="s">
+        <v>167</v>
+      </c>
+      <c r="G57" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="58" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A58" s="1" t="s">
         <v>35</v>
       </c>
@@ -2493,8 +2895,14 @@
       <c r="D58" s="1">
         <v>2</v>
       </c>
-    </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="F58" t="s">
+        <v>167</v>
+      </c>
+      <c r="G58" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="59" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A59" s="1" t="s">
         <v>33</v>
       </c>
@@ -2507,8 +2915,14 @@
       <c r="D59" s="1">
         <v>2</v>
       </c>
-    </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="F59" t="s">
+        <v>153</v>
+      </c>
+      <c r="G59" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="60" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A60" s="1" t="s">
         <v>31</v>
       </c>
@@ -2521,8 +2935,14 @@
       <c r="D60" s="1">
         <v>2</v>
       </c>
-    </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="F60" t="s">
+        <v>167</v>
+      </c>
+      <c r="G60" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="61" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A61" s="1" t="s">
         <v>29</v>
       </c>
@@ -2535,8 +2955,14 @@
       <c r="D61" s="1">
         <v>2</v>
       </c>
-    </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="F61" t="s">
+        <v>153</v>
+      </c>
+      <c r="G61" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="62" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A62" s="1" t="s">
         <v>27</v>
       </c>
@@ -2549,8 +2975,14 @@
       <c r="D62" s="1">
         <v>2</v>
       </c>
-    </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="F62" t="s">
+        <v>161</v>
+      </c>
+      <c r="G62" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="63" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A63" s="1" t="s">
         <v>25</v>
       </c>
@@ -2563,8 +2995,14 @@
       <c r="D63" s="1">
         <v>2</v>
       </c>
-    </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="F63" t="s">
+        <v>167</v>
+      </c>
+      <c r="G63" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="64" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A64" s="1" t="s">
         <v>23</v>
       </c>
@@ -2577,8 +3015,14 @@
       <c r="D64" s="1">
         <v>3</v>
       </c>
-    </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="F64" t="s">
+        <v>155</v>
+      </c>
+      <c r="G64" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="65" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A65" s="1" t="s">
         <v>21</v>
       </c>
@@ -2591,8 +3035,14 @@
       <c r="D65" s="1">
         <v>3</v>
       </c>
-    </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="F65" t="s">
+        <v>153</v>
+      </c>
+      <c r="G65" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="66" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A66" s="1" t="s">
         <v>19</v>
       </c>
@@ -2605,8 +3055,14 @@
       <c r="D66" s="1">
         <v>3</v>
       </c>
-    </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="F66" t="s">
+        <v>153</v>
+      </c>
+      <c r="G66" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="67" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A67" s="1" t="s">
         <v>17</v>
       </c>
@@ -2619,8 +3075,14 @@
       <c r="D67" s="1">
         <v>3</v>
       </c>
-    </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="F67" t="s">
+        <v>153</v>
+      </c>
+      <c r="G67" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="68" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A68" s="1" t="s">
         <v>15</v>
       </c>
@@ -2633,8 +3095,14 @@
       <c r="D68" s="1">
         <v>3</v>
       </c>
-    </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="F68" t="s">
+        <v>161</v>
+      </c>
+      <c r="G68" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="69" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A69" s="1" t="s">
         <v>13</v>
       </c>
@@ -2647,8 +3115,14 @@
       <c r="D69" s="1">
         <v>3</v>
       </c>
-    </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="F69" t="s">
+        <v>163</v>
+      </c>
+      <c r="G69" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="70" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A70" s="1" t="s">
         <v>11</v>
       </c>
@@ -2661,8 +3135,14 @@
       <c r="D70" s="1">
         <v>3</v>
       </c>
-    </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="F70" t="s">
+        <v>155</v>
+      </c>
+      <c r="G70" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="71" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A71" s="1" t="s">
         <v>9</v>
       </c>
@@ -2675,8 +3155,14 @@
       <c r="D71" s="1">
         <v>3</v>
       </c>
-    </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="F71" t="s">
+        <v>161</v>
+      </c>
+      <c r="G71" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="72" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A72" s="1" t="s">
         <v>7</v>
       </c>
@@ -2689,8 +3175,14 @@
       <c r="D72" s="1">
         <v>4</v>
       </c>
-    </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="F72" t="s">
+        <v>155</v>
+      </c>
+      <c r="G72" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="73" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A73" s="1" t="s">
         <v>5</v>
       </c>
@@ -2703,8 +3195,14 @@
       <c r="D73" s="1">
         <v>4</v>
       </c>
-    </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="F73" t="s">
+        <v>161</v>
+      </c>
+      <c r="G73" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="74" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A74" s="1" t="s">
         <v>3</v>
       </c>
@@ -2717,8 +3215,14 @@
       <c r="D74" s="1">
         <v>4</v>
       </c>
-    </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="F74" t="s">
+        <v>155</v>
+      </c>
+      <c r="G74" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="75" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A75" s="1" t="s">
         <v>1</v>
       </c>
@@ -2730,10 +3234,17 @@
       </c>
       <c r="D75" s="1">
         <v>4</v>
+      </c>
+      <c r="F75" t="s">
+        <v>167</v>
+      </c>
+      <c r="G75" t="s">
+        <v>168</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>